<commit_message>
can check for votes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E2B5EF-184C-4D38-B16A-9843EF64A957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Formulärsvar 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Formulärsvar 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -43,17 +52,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -63,40 +73,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -286,28 +301,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="39.71"/>
-    <col customWidth="1" min="5" max="10" width="21.57"/>
+    <col min="1" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -321,12 +339,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>43864.71445626157</v>
+        <v>43864.714456261572</v>
       </c>
       <c r="B2" s="3">
-        <v>111111.0</v>
+        <v>111111</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -335,12 +353,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43864.7146005324</v>
+        <v>43864.714600532403</v>
       </c>
       <c r="B3" s="3">
-        <v>222222.0</v>
+        <v>222222</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -349,12 +367,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>43864.71474773149</v>
+        <v>43864.714747731487</v>
       </c>
       <c r="B4" s="3">
-        <v>333333.0</v>
+        <v>333333</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -363,12 +381,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>43864.71522559028</v>
+        <v>43864.715225590277</v>
       </c>
       <c r="B5" s="3">
-        <v>222222.0</v>
+        <v>222222</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -377,7 +395,12 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can get all current elections
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A06C0-9FC7-40D7-8CCA-59B184D7C432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C0ADC0-D204-4F31-8B5F-353F5E82E77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Tidstämpel</t>
   </si>
@@ -28,12 +28,6 @@
     <t>Valkod</t>
   </si>
   <si>
-    <t>Val av Qurator</t>
-  </si>
-  <si>
-    <t>Val av Novischförman</t>
-  </si>
-  <si>
     <t>Alternativ 1</t>
   </si>
   <si>
@@ -47,6 +41,15 @@
   </si>
   <si>
     <t>Alternativ 3, Vakant 1, Vakant 2</t>
+  </si>
+  <si>
+    <t>Qurator</t>
+  </si>
+  <si>
+    <t>Novischförman</t>
+  </si>
+  <si>
+    <t>PQE</t>
   </si>
 </sst>
 </file>
@@ -311,11 +314,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -325,7 +328,7 @@
     <col min="5" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -333,13 +336,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43864.714456261572</v>
       </c>
@@ -347,13 +353,13 @@
         <v>111111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43864.714600532403</v>
       </c>
@@ -361,13 +367,13 @@
         <v>222222</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43864.714747731487</v>
       </c>
@@ -375,13 +381,13 @@
         <v>333333</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43864.715225590277</v>
       </c>
@@ -389,21 +395,21 @@
         <v>222222</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>123456</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can get all votes from columns
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C0ADC0-D204-4F31-8B5F-353F5E82E77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8A6778-4B31-49B7-92C0-3C4FBBD39399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,7 +318,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
almost finished with basic functionality of script
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC46FAE1-1F21-4A9E-A1DA-26C43DBA02C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5027187E-D3F1-41A6-BD64-18EAF1F35974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Tidstämpel</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Qurator</t>
   </si>
   <si>
-    <t>Novischförman</t>
-  </si>
-  <si>
     <t>PQE</t>
   </si>
   <si>
@@ -43,12 +40,6 @@
     <t>Qurator: Alternativ 2</t>
   </si>
   <si>
-    <t>Novischförman: Alternativ 2, Novischförman: Alternativ 3,  Novischförman: Vakant 1</t>
-  </si>
-  <si>
-    <t>Novischförman: Alternativ 1, Novischförman: Alternativ 2, Novischförman: Alternativ 3</t>
-  </si>
-  <si>
     <t>PQE: Alternativ 1</t>
   </si>
   <si>
@@ -56,9 +47,6 @@
   </si>
   <si>
     <t>PQE: Alternativ 3</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>Qurator: Alternativ Röv</t>
@@ -326,21 +314,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1"/>
-    <col min="5" max="10" width="21.5703125" customWidth="1"/>
+    <col min="1" max="9" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -350,14 +336,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43864.714456261572</v>
       </c>
@@ -365,16 +348,13 @@
         <v>111111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43864.714600532403</v>
       </c>
@@ -382,16 +362,13 @@
         <v>222222</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43864.714747731487</v>
       </c>
@@ -399,16 +376,13 @@
         <v>333333</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43864.715225590277</v>
       </c>
@@ -416,35 +390,28 @@
         <v>222222</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>123456</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nested voting almost works
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5027187E-D3F1-41A6-BD64-18EAF1F35974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Formulärsvar 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Formulärsvar 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Tidstämpel</t>
   </si>
@@ -34,87 +25,100 @@
     <t>PQE</t>
   </si>
   <si>
+    <t>Novischförman</t>
+  </si>
+  <si>
     <t>Qurator: Alternativ 1</t>
   </si>
   <si>
+    <t>PQE: Alternativ 1</t>
+  </si>
+  <si>
+    <t>Novischförman: Alternativ 1, Novischförman: Alternativ 2, Novischförman: Alternativ 3</t>
+  </si>
+  <si>
+    <t>Novischförman: Alternativ 1, Novischförman: Alternativ 2, Novischförman: Vakant</t>
+  </si>
+  <si>
     <t>Qurator: Alternativ 2</t>
   </si>
   <si>
-    <t>PQE: Alternativ 1</t>
+    <t>PQE: Vakant</t>
+  </si>
+  <si>
+    <t>Novischförman: Alternativ 3, Novischförman: Vakant, Novischförman: Blankt</t>
   </si>
   <si>
     <t>PQE: Alternativ 2</t>
   </si>
   <si>
-    <t>PQE: Alternativ 3</t>
-  </si>
-  <si>
-    <t>Qurator: Alternativ Röv</t>
+    <t>Novischförman: Blankt</t>
+  </si>
+  <si>
+    <t>Qurator: Blankt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -304,114 +308,147 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="9" width="21.5703125" customWidth="1"/>
+    <col customWidth="1" min="1" max="5" width="21.57"/>
+    <col customWidth="1" min="6" max="6" width="39.71"/>
+    <col customWidth="1" min="7" max="12" width="21.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>43864.714456261572</v>
-      </c>
-      <c r="B2" s="3">
-        <v>111111</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>43917.92002694444</v>
+      </c>
+      <c r="B2" s="4">
+        <v>111111.0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>43864.714600532403</v>
-      </c>
-      <c r="B3" s="3">
-        <v>222222</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>43864.714747731487</v>
-      </c>
-      <c r="B4" s="3">
-        <v>333333</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="3">
+      <c r="A3" s="3">
+        <v>43917.92015318287</v>
+      </c>
+      <c r="B3" s="4">
+        <v>222222.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>43917.920314884264</v>
+      </c>
+      <c r="B4" s="4">
+        <v>333333.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>43917.92051686342</v>
+      </c>
+      <c r="B5" s="4">
+        <v>111111.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>43917.92096502315</v>
+      </c>
+      <c r="B6" s="4">
+        <v>333333.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>43864.715225590277</v>
-      </c>
-      <c r="B5" s="3">
-        <v>222222</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
-        <v>123456</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="7">
+      <c r="A7" s="3">
+        <v>43917.921102754626</v>
+      </c>
+      <c r="B7" s="4">
+        <v>777777.0</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
firebase setup - sketch fest
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Tidstämpel</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Qurator: Blankt</t>
+  </si>
+  <si>
+    <t>Novischförman: Alternativ 1, Novischförman: Alternativ 2, Novischförman: Blankt</t>
   </si>
 </sst>
 </file>
@@ -448,6 +451,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>43917.98333636574</v>
+      </c>
+      <c r="B8" s="4">
+        <v>123456.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>